<commit_message>
Added excel files acting as patient database
</commit_message>
<xml_diff>
--- a/patient.xlsx
+++ b/patient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorby\Desktop\Diary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8761642D-81C3-4A63-BDB3-34F28E5864A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C19735-0D61-418E-9F81-C10EE3E8B058}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="18000" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>****</t>
   </si>
   <si>
-    <t>Ashok Gupta</t>
-  </si>
-  <si>
     <t>Manish Kumar</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>['Dry Cough']</t>
+  </si>
+  <si>
+    <t>Janhvi Tripathi</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -657,7 +659,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -665,52 +667,52 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -718,52 +720,52 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -771,52 +773,52 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -824,52 +826,52 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -877,52 +879,52 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -930,52 +932,52 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -983,52 +985,52 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
         <v>39</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>39</v>
       </c>
-      <c r="J9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" t="s">
-        <v>40</v>
-      </c>
       <c r="L9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1036,52 +1038,52 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1089,52 +1091,52 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1142,52 +1144,52 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Password based authentication
SHA256 hashing based dataset for user passwords
</commit_message>
<xml_diff>
--- a/patient.xlsx
+++ b/patient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorby\Desktop\Diary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C19735-0D61-418E-9F81-C10EE3E8B058}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6E4BCF-4C0C-4334-AB82-83D606522BCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="18000" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -28,6 +28,9 @@
     <t>name</t>
   </si>
   <si>
+    <t>password</t>
+  </si>
+  <si>
     <t>age</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>****</t>
   </si>
   <si>
+    <t>Janhvi Tripathi</t>
+  </si>
+  <si>
     <t>Manish Kumar</t>
   </si>
   <si>
@@ -103,6 +109,9 @@
     <t>Priyesh Bhawsar</t>
   </si>
   <si>
+    <t>5e884898da28047151d0e56f8dc6292773603d0d6aabbdd62a11ef721d1542d8</t>
+  </si>
+  <si>
     <t>**</t>
   </si>
   <si>
@@ -176,9 +185,6 @@
   </si>
   <si>
     <t>['Dry Cough']</t>
-  </si>
-  <si>
-    <t>Janhvi Tripathi</t>
   </si>
 </sst>
 </file>
@@ -580,25 +586,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" customWidth="1"/>
-    <col min="7" max="7" width="43.28515625" customWidth="1"/>
-    <col min="8" max="8" width="45.42578125" customWidth="1"/>
-    <col min="9" max="9" width="43.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,107 +646,110 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
         <v>65</v>
       </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="O3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="Q3" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="R3" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="M4" t="s">
         <v>44</v>
@@ -759,437 +758,440 @@
         <v>47</v>
       </c>
       <c r="O4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q4" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="R4" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q5" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" t="s">
-        <v>28</v>
-      </c>
       <c r="M6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="O6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="P6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="Q6" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="R6" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
         <v>64</v>
       </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="L7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="M7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="N7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="P7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="Q7" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="R7" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
-        <v>30</v>
+      <c r="D8">
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="P8" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="Q8" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="R8" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9">
+        <v>25</v>
+      </c>
+      <c r="D9">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N9" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="O9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q9" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="R9" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10">
+        <v>26</v>
+      </c>
+      <c r="D10">
         <v>48</v>
       </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
         <v>47</v>
       </c>
       <c r="L10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q10" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="R10" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N11" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="O11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q11" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="R11" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
+        <v>28</v>
+      </c>
+      <c r="D12">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="M12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="N12" t="s">
         <v>51</v>
       </c>
       <c r="O12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="P12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="Q12" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="R12" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>